<commit_message>
feat: add separate analysis for elderly and non elderly
</commit_message>
<xml_diff>
--- a/tables/table_100k_rates_2019_2021.xlsx
+++ b/tables/table_100k_rates_2019_2021.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1213,6 +1213,254 @@
         <v>-51.70940170940172</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Admissions_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>-26.2181808947216</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-26.92994131880578</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-25.49948735862907</v>
+      </c>
+      <c r="F26" t="n">
+        <v>801</v>
+      </c>
+      <c r="G26" t="n">
+        <v>533</v>
+      </c>
+      <c r="H26" t="n">
+        <v>445</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-44.44444444444444</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Admissions_non_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>-17.21045888725881</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-17.73862587488443</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-16.6789007531834</v>
+      </c>
+      <c r="F27" t="n">
+        <v>88</v>
+      </c>
+      <c r="G27" t="n">
+        <v>73</v>
+      </c>
+      <c r="H27" t="n">
+        <v>61</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-30.68181818181818</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Admissions_uti_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>-7.700048924177882</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-10.66947333950832</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-4.631918258162604</v>
+      </c>
+      <c r="F28" t="n">
+        <v>53</v>
+      </c>
+      <c r="G28" t="n">
+        <v>54</v>
+      </c>
+      <c r="H28" t="n">
+        <v>45</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-15.09433962264151</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Admissions_uti_non_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2.985009492824675</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.731746798459687</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5.288675291783629</v>
+      </c>
+      <c r="F29" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7</v>
+      </c>
+      <c r="H29" t="n">
+        <v>6</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Admissions_non_uti_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>-27.7717156328871</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-28.50203645568175</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-27.03393489826046</v>
+      </c>
+      <c r="F30" t="n">
+        <v>749</v>
+      </c>
+      <c r="G30" t="n">
+        <v>480</v>
+      </c>
+      <c r="H30" t="n">
+        <v>400</v>
+      </c>
+      <c r="I30" t="n">
+        <v>-46.5954606141522</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Admissions_non_uti_non_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>-18.8390345105688</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-19.38049573696554</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-18.29393669198049</v>
+      </c>
+      <c r="F31" t="n">
+        <v>83</v>
+      </c>
+      <c r="G31" t="n">
+        <v>66</v>
+      </c>
+      <c r="H31" t="n">
+        <v>55</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-33.73493975903614</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Mortality_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>-14.51407613111556</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-16.19542779828318</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-12.79899189596965</v>
+      </c>
+      <c r="F32" t="n">
+        <v>160</v>
+      </c>
+      <c r="G32" t="n">
+        <v>135</v>
+      </c>
+      <c r="H32" t="n">
+        <v>117</v>
+      </c>
+      <c r="I32" t="n">
+        <v>-26.875</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Mortality_non_eld_Tx</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>-3.967703623114516</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-5.928045253893643</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-1.966510929765908</v>
+      </c>
+      <c r="F33" t="n">
+        <v>8</v>
+      </c>
+      <c r="G33" t="n">
+        <v>8</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-12.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>